<commit_message>
week12 notes on temporary diff using q
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/week12/temporary-difference.xlsx
+++ b/week12/temporary-difference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\ECID2\rl\week12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DFDE71-1633-426D-88DF-6123B3ACD3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB34AA6-3D12-45CB-A3E3-A18176A4E6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{76B46E62-252C-4031-B4FC-38427F8B6B71}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="20">
   <si>
     <t>s1</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>s→sf</t>
   </si>
   <si>
     <t>Transition Model</t>
@@ -143,7 +140,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,9 +256,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1161,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307D8DED-F681-4012-9DD2-D8D3828C92F8}">
   <dimension ref="B3:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1160,7 @@
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>3</v>
@@ -1291,9 +1279,6 @@
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
-      <c r="Q6" s="21" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
@@ -1330,7 +1315,7 @@
         <v>0.2</v>
       </c>
       <c r="N7" s="17">
-        <v>-7.3975999999999997</v>
+        <v>8.9969999999999999</v>
       </c>
       <c r="O7" s="2">
         <v>0.14000000000000001</v>
@@ -1352,19 +1337,19 @@
         <v>12</v>
       </c>
       <c r="M8" s="3">
-        <v>0.24199999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="N8" s="17">
-        <v>0.57399999999999995</v>
+        <v>0.15</v>
       </c>
       <c r="O8" s="17">
-        <v>0.51319999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="P8" s="17">
-        <v>8.7477999999999998</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="Q8" s="4">
-        <v>8.8187999999999995</v>
+        <v>0.89</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>4</v>
@@ -1393,7 +1378,7 @@
       <c r="F10" s="1">
         <v>0.8</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="L11" s="7" t="s">
@@ -1401,10 +1386,6 @@
       </c>
       <c r="M11" s="1">
         <v>0.9</v>
-      </c>
-      <c r="N11">
-        <f>Q8+M12*((Q5+M11*MAX(Q7,Q8)) - Q8)</f>
-        <v>16.113296000000002</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">

</xml_diff>